<commit_message>
Updated Tutorial and Changed Fish Size
</commit_message>
<xml_diff>
--- a/Jetpack/Assets/Resources/Patterns/Fish/fish_patterns.xlsx
+++ b/Jetpack/Assets/Resources/Patterns/Fish/fish_patterns.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding Projects\School\ecs189L\back-to-the-jungle\Jetpack\Assets\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding Projects\School\ecs189L\back-to-the-jungle\Jetpack\Assets\Resources\Patterns\Fish\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3108EC9D-6B6A-43AD-AC8B-65BBD39C1F70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D3FFCE-1B5F-47EE-B54D-15A78F2D1BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{D6B53B84-B4B8-429A-BFC6-3A192A739905}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="10" xr2:uid="{D6B53B84-B4B8-429A-BFC6-3A192A739905}"/>
   </bookViews>
   <sheets>
     <sheet name="BEAN" sheetId="2" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="Big Arrow" sheetId="14" r:id="rId8"/>
     <sheet name="Small Arrows" sheetId="15" r:id="rId9"/>
     <sheet name="Smile" sheetId="17" r:id="rId10"/>
+    <sheet name="Smile (2)" sheetId="19" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>D6</t>
   </si>
@@ -72,6 +73,12 @@
   </si>
   <si>
     <t>M3</t>
+  </si>
+  <si>
+    <t>F5</t>
+  </si>
+  <si>
+    <t>T3</t>
   </si>
 </sst>
 </file>
@@ -146,8 +153,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF0000"/>
       <color rgb="FF0D0D0D"/>
-      <color rgb="FFFF0000"/>
     </mruColors>
   </colors>
   <extLst>
@@ -572,6 +579,51 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2DAF8F2-41C7-47A5-BBFC-A05A8FF9B712}">
+  <dimension ref="A1:T5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.28515625" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="S3" s="4"/>
+    </row>
+    <row r="4" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F4" s="2"/>
+      <c r="H4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="T4" s="4"/>
+    </row>
+    <row r="5" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="S5" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFC77F05-1BB9-4B99-BEC3-72145FA551A3}">
   <dimension ref="A1:H6"/>
@@ -644,7 +696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E6A6877-C119-4BD2-8E74-B92AB35BE0E2}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>

</xml_diff>